<commit_message>
Se agregaron al script reg_so, las caidas acumuladas de las variables  market share e industria
</commit_message>
<xml_diff>
--- a/output/table_recession.xlsx
+++ b/output/table_recession.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresmarticorenavidal/Investigacion/Ayudantia_Angel/mobile_so_project/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{145DABD7-58BB-9C4C-A09C-0DD0E015EAA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E9BFAC-5ACF-F64C-81E4-4236A29808AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21600" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{054FE367-16C3-C843-8732-BC38582AF50E}"/>
+    <workbookView xWindow="21600" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{054FE367-16C3-C843-8732-BC38582AF50E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="60">
   <si>
     <t xml:space="preserve">Country </t>
   </si>
@@ -204,7 +204,16 @@
     <t>United States</t>
   </si>
   <si>
-    <t>*NOTA: Países sin recesión no son considerados en la tabla. La caída acumulada se calculo tomando el periodo de inicio de la recesión versus el último trimestre de  recesión</t>
+    <t>Caida Acumulada Industria</t>
+  </si>
+  <si>
+    <t>Caida Acumulada Market share Andriod</t>
+  </si>
+  <si>
+    <t>Caida Acumulada Market share iOS</t>
+  </si>
+  <si>
+    <t>*NOTA: Países sin recesión no son considerados en la tabla. La caída acumulada se calculo tomando el periodo de inicio de la recesión versus el último trimestre de  recesión. País en gris se debe a que no hay fecha en el panel de termino de la recesión</t>
   </si>
 </sst>
 </file>
@@ -227,12 +236,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -268,7 +283,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -281,6 +296,11 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1AC7A13-19B1-2342-BB88-E35CFA632694}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -608,9 +628,12 @@
     <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -623,8 +646,18 @@
       <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -637,8 +670,17 @@
       <c r="D2" s="2">
         <v>-3.204347E-4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="2">
+        <v>9.4827919999999996E-2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2">
+        <v>-0.48237269999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -651,16 +693,29 @@
       <c r="D3" s="2">
         <v>-4.15428932E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="E3" s="2">
+        <v>0.1117717</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.24907940000000001</v>
+      </c>
+      <c r="G3" s="2">
+        <v>-0.1994638</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="14">
         <v>43101</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -673,8 +728,17 @@
       <c r="D5" s="2">
         <v>7.706789E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="2">
+        <v>1.3291591E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>8.75</v>
+      </c>
+      <c r="G5" s="2">
+        <v>-0.27640199999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -687,8 +751,17 @@
       <c r="D6" s="2">
         <v>3.3549559999999999E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="2">
+        <v>3.7994930000000001E-3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>8.1889160000000003E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>-6.3895300000000002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -701,8 +774,17 @@
       <c r="D7" s="2">
         <v>3.5546469999999997E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="2">
+        <v>-1.7222629999999999E-3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>124.63639999999999</v>
+      </c>
+      <c r="G7" s="2">
+        <v>3.4098709999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -715,8 +797,17 @@
       <c r="D8" s="2">
         <v>0.10319221000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="2">
+        <v>-5.6547148999999998E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>24.857142856999999</v>
+      </c>
+      <c r="G8" s="2">
+        <v>-0.1246543</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -729,8 +820,17 @@
       <c r="D9" s="2">
         <v>-0.18046620999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="2">
+        <v>-1.095782E-3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>67.060483871000002</v>
+      </c>
+      <c r="G9" s="2">
+        <v>-0.28437896099999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -743,8 +843,17 @@
       <c r="D10" s="2">
         <v>9.0034169999999997E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="2">
+        <v>7.939293E-3</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2.8761540000000001E-3</v>
+      </c>
+      <c r="G10" s="2">
+        <v>6.6033840000000003E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -757,8 +866,17 @@
       <c r="D11" s="2">
         <v>6.4892561000000001E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="2">
+        <v>6.4176731000000001E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>25.764705880000001</v>
+      </c>
+      <c r="G11" s="2">
+        <v>7.9363810000000007E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -771,8 +889,17 @@
       <c r="D12" s="2">
         <v>-7.9970211999999999E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="2">
+        <v>9.2133830000000003E-3</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.33353316999999999</v>
+      </c>
+      <c r="G12" s="2">
+        <v>8.2533229999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -785,8 +912,17 @@
       <c r="D13" s="2">
         <v>-6.9084769999999997E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="2">
+        <v>-5.0354531000000001E-2</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.51005025000000004</v>
+      </c>
+      <c r="G13" s="2">
+        <v>-0.28486006000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -799,8 +935,17 @@
       <c r="D14" s="2">
         <v>0.122007427</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="2">
+        <v>-2.5603240000000001E-3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3.0258259999999999E-2</v>
+      </c>
+      <c r="G14" s="2">
+        <v>-2.600763E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -813,8 +958,17 @@
       <c r="D15" s="2">
         <v>8.0596630000000002E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="2">
+        <v>0.15510450000000001</v>
+      </c>
+      <c r="F15" s="2">
+        <v>7.6</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.16866585000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -827,8 +981,17 @@
       <c r="D16" s="2">
         <v>-4.9368219999999997E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="2">
+        <v>2.032014E-2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1.486035E-2</v>
+      </c>
+      <c r="G16" s="2">
+        <v>-4.7920789999999998E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -841,8 +1004,17 @@
       <c r="D17" s="2">
         <v>-5.4088820000000003E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="2">
+        <v>4.5706919999999998E-2</v>
+      </c>
+      <c r="F17" s="2">
+        <v>110.375</v>
+      </c>
+      <c r="G17" s="2">
+        <v>5.3092029999999998E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -855,8 +1027,17 @@
       <c r="D18" s="2">
         <v>1.4157803E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="2">
+        <v>1.43213E-2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.74884170000000005</v>
+      </c>
+      <c r="G18" s="2">
+        <v>-1.2197380000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -869,8 +1050,17 @@
       <c r="D19" s="2">
         <v>-1.0975260000000001E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="2">
+        <v>-6.0419861999999998E-2</v>
+      </c>
+      <c r="F19" s="2">
+        <v>102.52941176</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1.6504899999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -883,8 +1073,17 @@
       <c r="D20" s="2">
         <v>-5.0418770000000002E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="2">
+        <v>-9.2160950000000005E-3</v>
+      </c>
+      <c r="F20" s="2">
+        <v>-7.9664979999999996E-2</v>
+      </c>
+      <c r="G20" s="2">
+        <v>4.5990499999999997E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -897,8 +1096,17 @@
       <c r="D21" s="2">
         <v>-3.2497779999999997E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="2">
+        <v>-2.4381150000000001E-2</v>
+      </c>
+      <c r="F21" s="2">
+        <v>13.98333</v>
+      </c>
+      <c r="G21" s="2">
+        <v>-0.53092419999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -911,8 +1119,17 @@
       <c r="D22" s="2">
         <v>-1.125351E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="2">
+        <v>1.024071E-2</v>
+      </c>
+      <c r="F22" s="2">
+        <v>32.1</v>
+      </c>
+      <c r="G22" s="2">
+        <v>-0.1834462</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -925,8 +1142,17 @@
       <c r="D23" s="2">
         <v>-2.2238850000000001E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="2">
+        <v>3.6874589999999999E-2</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.42871700000000001</v>
+      </c>
+      <c r="G23" s="2">
+        <v>-6.9972270000000003E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -939,8 +1165,17 @@
       <c r="D24" s="2">
         <v>0.14051547</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="2">
+        <v>2.277464E-4</v>
+      </c>
+      <c r="F24" s="2">
+        <v>71</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.16914286000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -953,8 +1188,17 @@
       <c r="D25" s="2">
         <v>2.5667829999999999E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="2">
+        <v>1.6587035E-3</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.10293568</v>
+      </c>
+      <c r="G25" s="2">
+        <v>-2.404719E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -967,8 +1211,17 @@
       <c r="D26" s="2">
         <v>4.5040660000000003E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" s="2">
+        <v>-5.1165797999999998E-3</v>
+      </c>
+      <c r="F26" s="2">
+        <v>2.840353E-2</v>
+      </c>
+      <c r="G26" s="2">
+        <v>-3.8692709999999998E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -981,8 +1234,17 @@
       <c r="D27" s="2">
         <v>7.2890919999999998E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" s="2">
+        <v>5.9519099999999998E-2</v>
+      </c>
+      <c r="F27" s="2">
+        <v>16.125</v>
+      </c>
+      <c r="G27" s="2">
+        <v>-0.35767330000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -995,8 +1257,17 @@
       <c r="D28" s="2">
         <v>6.7042180000000007E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" s="2">
+        <v>2.1887029999999998E-2</v>
+      </c>
+      <c r="F28" s="2">
+        <v>-0.84375</v>
+      </c>
+      <c r="G28" s="2">
+        <v>2.979826E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -1009,16 +1280,29 @@
       <c r="D29" s="2">
         <v>9.4826779999999999E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="E29" s="2">
+        <v>4.7490709999999998E-2</v>
+      </c>
+      <c r="F29" s="2">
+        <v>13.25</v>
+      </c>
+      <c r="G29" s="2">
+        <v>-0.16249040000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="14">
         <v>43647</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -1031,8 +1315,17 @@
       <c r="D31" s="2">
         <v>-2.1870890000000001E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" s="2">
+        <v>2.633191E-2</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.73684210000000006</v>
+      </c>
+      <c r="G31" s="2">
+        <v>-4.3278949999999997E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -1045,8 +1338,17 @@
       <c r="D32" s="2">
         <v>5.889382E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" s="2">
+        <v>3.02656E-2</v>
+      </c>
+      <c r="F32" s="2">
+        <v>21.428570000000001</v>
+      </c>
+      <c r="G32" s="2">
+        <v>-0.14189640000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1059,8 +1361,17 @@
       <c r="D33" s="2">
         <v>-5.0461579999999999E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" s="2">
+        <v>-8.9313470000000006E-2</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1.4312800000000001</v>
+      </c>
+      <c r="G33" s="2">
+        <v>-0.37515330000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1073,8 +1384,17 @@
       <c r="D34" s="2">
         <v>1.327212E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" s="2">
+        <v>8.4364839999999993E-3</v>
+      </c>
+      <c r="F34" s="2">
+        <v>86.68571</v>
+      </c>
+      <c r="G34" s="2">
+        <v>-4.1165930000000003E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1087,8 +1407,17 @@
       <c r="D35" s="2">
         <v>2.3273329999999998E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" s="2">
+        <v>1.399983E-3</v>
+      </c>
+      <c r="F35" s="2">
+        <v>50.125</v>
+      </c>
+      <c r="G35" s="2">
+        <v>-0.45536100000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1101,8 +1430,17 @@
       <c r="D36" s="2">
         <v>9.6233860000000004E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" s="2">
+        <v>-7.3779340000000001E-3</v>
+      </c>
+      <c r="F36" s="2">
+        <v>4.8571429000000004</v>
+      </c>
+      <c r="G36" s="2">
+        <v>-0.43047920000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -1115,8 +1453,17 @@
       <c r="D37" s="2">
         <v>-6.6585770000000002E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" s="2">
+        <v>1.0909090999999999E-2</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.31706109999999998</v>
+      </c>
+      <c r="G37" s="2">
+        <v>-0.192361</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -1129,8 +1476,17 @@
       <c r="D38" s="2">
         <v>0.17037640000000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" s="2">
+        <v>7.5048019999999993E-2</v>
+      </c>
+      <c r="F38" s="2">
+        <v>9</v>
+      </c>
+      <c r="G38" s="2">
+        <v>-0.25589919999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -1143,8 +1499,17 @@
       <c r="D39" s="2">
         <v>0.43855820000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" s="2">
+        <v>-5.7569719999999998E-2</v>
+      </c>
+      <c r="F39" s="2">
+        <v>653.57140000000004</v>
+      </c>
+      <c r="G39" s="2">
+        <v>7.0915339999999993E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>25</v>
       </c>
@@ -1157,8 +1522,17 @@
       <c r="D40" s="2">
         <v>5.8373990000000001E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" s="2">
+        <v>1.4720240000000001E-2</v>
+      </c>
+      <c r="F40" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="G40" s="2">
+        <v>6.731558E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -1171,8 +1545,17 @@
       <c r="D41" s="2">
         <v>0.26683289900000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" s="2">
+        <v>-1.384167E-2</v>
+      </c>
+      <c r="F41" s="2">
+        <v>10.3333333</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0.79949022999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -1185,8 +1568,17 @@
       <c r="D42" s="2">
         <v>-6.262213E-3</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" s="2">
+        <v>1.499559E-2</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.75510509999999997</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0.59263195000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>26</v>
       </c>
@@ -1199,8 +1591,17 @@
       <c r="D43" s="2">
         <v>6.1095379999999998E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" s="2">
+        <v>-5.6428619999999999E-2</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.29361559999999998</v>
+      </c>
+      <c r="G43" s="2">
+        <v>-6.9413569999999994E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>27</v>
       </c>
@@ -1213,8 +1614,17 @@
       <c r="D44" s="2">
         <v>0.1129479</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" s="2">
+        <v>3.6297349999999999E-2</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1.6140350000000001</v>
+      </c>
+      <c r="G44" s="2">
+        <v>3.255077E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -1227,8 +1637,17 @@
       <c r="D45" s="2">
         <v>6.3378095999999995E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" s="2">
+        <v>6.5728679999999998E-2</v>
+      </c>
+      <c r="F45" s="2">
+        <v>20.8</v>
+      </c>
+      <c r="G45" s="2">
+        <v>-0.37129519999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>28</v>
       </c>
@@ -1241,8 +1660,17 @@
       <c r="D46" s="2">
         <v>-8.4368896999999998E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" s="2">
+        <v>3.4960239999999997E-2</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0.15686030000000001</v>
+      </c>
+      <c r="G46" s="2">
+        <v>-0.34908866</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>28</v>
       </c>
@@ -1255,8 +1683,17 @@
       <c r="D47" s="2">
         <v>-6.9533727000000004E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" s="2">
+        <v>-1.4721740000000001E-2</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0.23247789999999999</v>
+      </c>
+      <c r="G47" s="2">
+        <v>-0.23264852999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>28</v>
       </c>
@@ -1269,19 +1706,29 @@
       <c r="D48" s="2">
         <v>-5.1350010000000001E-3</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="E48" s="2">
+        <v>-2.8600219999999999E-2</v>
+      </c>
+      <c r="F48" s="2">
+        <v>8.77164E-2</v>
+      </c>
+      <c r="G48" s="2">
+        <v>1.082837E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="14">
         <v>43191</v>
       </c>
-      <c r="C49">
-        <v>9.6726599999999996E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>29</v>
       </c>
@@ -1294,8 +1741,17 @@
       <c r="D50" s="2">
         <v>4.5564280000000004E-3</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50" s="16">
+        <v>1.6084649999999999E-2</v>
+      </c>
+      <c r="F50" s="2">
+        <v>27.142857143000001</v>
+      </c>
+      <c r="G50" s="2">
+        <v>-8.2713969999999998E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>29</v>
       </c>
@@ -1308,8 +1764,17 @@
       <c r="D51" s="2">
         <v>-7.0549946000000002E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" s="16">
+        <v>3.6541549999999999E-5</v>
+      </c>
+      <c r="F51" s="2">
+        <v>-3.5730649999999998E-3</v>
+      </c>
+      <c r="G51" s="2">
+        <v>-5.9628859999999999E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>30</v>
       </c>
@@ -1322,8 +1787,17 @@
       <c r="D52" s="2">
         <v>0.16161765</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52" s="2">
+        <v>1.3947424E-2</v>
+      </c>
+      <c r="F52" s="2">
+        <v>19.076923099999998</v>
+      </c>
+      <c r="G52" s="2">
+        <v>-0.17122770000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>30</v>
       </c>
@@ -1336,8 +1810,17 @@
       <c r="D53" s="2">
         <v>-7.2362750000000003E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" s="2">
+        <v>7.0582900000000005E-4</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0.18174419999999999</v>
+      </c>
+      <c r="G53" s="2">
+        <v>-2.0850199999999999E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -1350,8 +1833,17 @@
       <c r="D54" s="2">
         <v>7.1439403400000004E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" s="2">
+        <v>2.7491959999999999E-2</v>
+      </c>
+      <c r="F54" s="2">
+        <v>8.5625</v>
+      </c>
+      <c r="G54" s="2">
+        <v>-0.10461303</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>31</v>
       </c>
@@ -1364,8 +1856,17 @@
       <c r="D55" s="2">
         <v>-4.603349E-4</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55" s="2">
+        <v>3.686917E-2</v>
+      </c>
+      <c r="F55" s="2">
+        <v>-2.6745219999999999E-3</v>
+      </c>
+      <c r="G55" s="2">
+        <v>-3.6370180000000002E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>32</v>
       </c>
@@ -1378,8 +1879,17 @@
       <c r="D56" s="2">
         <v>2.6656674000000002E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" s="16">
+        <v>2.6894410000000001E-2</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G56" s="2">
+        <v>0.85219400000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>32</v>
       </c>
@@ -1392,8 +1902,17 @@
       <c r="D57" s="2">
         <v>-7.6550719999999997E-3</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57" s="16">
+        <v>9.5529680000000002E-3</v>
+      </c>
+      <c r="F57" s="2">
+        <v>0.38945660999999998</v>
+      </c>
+      <c r="G57" s="2">
+        <v>1.833661E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>32</v>
       </c>
@@ -1406,8 +1925,17 @@
       <c r="D58" s="2">
         <v>-1.4018887000000001E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58" s="16">
+        <v>2.5930039999999999E-3</v>
+      </c>
+      <c r="F58" s="2">
+        <v>6.1985560000000002E-2</v>
+      </c>
+      <c r="G58" s="2">
+        <v>6.6627699999999998E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>32</v>
       </c>
@@ -1420,8 +1948,17 @@
       <c r="D59" s="2">
         <v>1.2855042000000001E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59" s="16">
+        <v>-2.3401230000000001E-5</v>
+      </c>
+      <c r="F59" s="2">
+        <v>1.6074990000000001E-2</v>
+      </c>
+      <c r="G59" s="2">
+        <v>-0.12694462000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>33</v>
       </c>
@@ -1434,8 +1971,17 @@
       <c r="D60" s="5">
         <v>0.26568247</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" s="2">
+        <v>-8.0440140000000004E-3</v>
+      </c>
+      <c r="F60" s="2">
+        <v>13</v>
+      </c>
+      <c r="G60" s="2">
+        <v>-0.32940009999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>33</v>
       </c>
@@ -1448,8 +1994,17 @@
       <c r="D61" s="2">
         <v>1.7573490000000001E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" s="2">
+        <v>6.6334519999999998E-3</v>
+      </c>
+      <c r="F61" s="2">
+        <v>1.6708400000000002E-2</v>
+      </c>
+      <c r="G61" s="2">
+        <v>-3.5372849999999997E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -1462,8 +2017,17 @@
       <c r="D62" s="2">
         <v>3.2270100000000003E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62" s="2">
+        <v>2.6407150000000001E-2</v>
+      </c>
+      <c r="F62" s="2">
+        <v>32.636364</v>
+      </c>
+      <c r="G62" s="2">
+        <v>-0.12914870000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>34</v>
       </c>
@@ -1476,8 +2040,17 @@
       <c r="D63" s="2">
         <v>-3.7802370000000002E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63" s="2">
+        <v>-2.1520230000000001E-2</v>
+      </c>
+      <c r="F63" s="2">
+        <v>1.516049</v>
+      </c>
+      <c r="G63" s="2">
+        <v>0.15279609999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>35</v>
       </c>
@@ -1490,8 +2063,17 @@
       <c r="D64" s="2">
         <v>5.4157499999999997E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" s="2">
+        <v>-0.11857143000000001</v>
+      </c>
+      <c r="F64" s="2">
+        <v>5.5506329000000001</v>
+      </c>
+      <c r="G64" s="2">
+        <v>-0.10150247</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>35</v>
       </c>
@@ -1504,8 +2086,17 @@
       <c r="D65" s="2">
         <v>-2.9637030000000002E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" s="2">
+        <v>3.9670740000000003E-2</v>
+      </c>
+      <c r="F65" s="2">
+        <v>0.15629850000000001</v>
+      </c>
+      <c r="G65" s="2">
+        <v>-9.9489129999999995E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>36</v>
       </c>
@@ -1518,8 +2109,17 @@
       <c r="D66" s="2">
         <v>0.13692409999999999</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66" s="2">
+        <v>5.8290979999999999E-2</v>
+      </c>
+      <c r="F66" s="2">
+        <v>29.33333</v>
+      </c>
+      <c r="G66" s="2">
+        <v>-0.4873015</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>37</v>
       </c>
@@ -1532,8 +2132,17 @@
       <c r="D67" s="2">
         <v>-2.735782E-3</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" s="2">
+        <v>-6.4406420000000003E-4</v>
+      </c>
+      <c r="F67" s="2">
+        <v>11.461538462</v>
+      </c>
+      <c r="G67" s="2">
+        <v>0.108865061</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>37</v>
       </c>
@@ -1546,8 +2155,17 @@
       <c r="D68" s="2">
         <v>1.3519194999999999E-2</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" s="2">
+        <v>5.3806538000000003E-3</v>
+      </c>
+      <c r="F68" s="2">
+        <v>8.4167474000000006E-2</v>
+      </c>
+      <c r="G68" s="2">
+        <v>-9.0893689999999999E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>37</v>
       </c>
@@ -1560,8 +2178,17 @@
       <c r="D69" s="2">
         <v>3.0888476000000002E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" s="2">
+        <v>1.6303712999999999E-3</v>
+      </c>
+      <c r="F69" s="2">
+        <v>-7.8920569999999992E-3</v>
+      </c>
+      <c r="G69" s="2">
+        <v>6.163328E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>38</v>
       </c>
@@ -1574,8 +2201,17 @@
       <c r="D70" s="2">
         <v>-3.55208E-3</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70" s="2">
+        <v>-4.8141349999999999E-2</v>
+      </c>
+      <c r="F70" s="2">
+        <v>3.3959044</v>
+      </c>
+      <c r="G70" s="2">
+        <v>1.4351928999999999E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>38</v>
       </c>
@@ -1588,8 +2224,17 @@
       <c r="D71" s="2">
         <v>-1.0782409999999999E-2</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71" s="2">
+        <v>-1.288043E-2</v>
+      </c>
+      <c r="F71" s="2">
+        <v>0.17371529999999999</v>
+      </c>
+      <c r="G71" s="2">
+        <v>1.0735759999999999E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>39</v>
       </c>
@@ -1602,8 +2247,17 @@
       <c r="D72" s="2">
         <v>-4.1129749999999996E-3</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72" s="2">
+        <v>5.7849396999999997E-2</v>
+      </c>
+      <c r="F72" s="2">
+        <v>17.079999999999998</v>
+      </c>
+      <c r="G72" s="2">
+        <v>-0.26262990000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>39</v>
       </c>
@@ -1616,8 +2270,17 @@
       <c r="D73" s="2">
         <v>-0.12297677999999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73" s="2">
+        <v>9.1739790000000005E-3</v>
+      </c>
+      <c r="F73" s="2">
+        <v>1.4524649999999999</v>
+      </c>
+      <c r="G73" s="2">
+        <v>-0.39713989999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>40</v>
       </c>
@@ -1630,8 +2293,17 @@
       <c r="D74" s="2">
         <v>7.5090169999999998E-2</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74" s="2">
+        <v>-1.0660080000000001E-2</v>
+      </c>
+      <c r="F74" s="2">
+        <v>16.625</v>
+      </c>
+      <c r="G74" s="2">
+        <v>-0.32504909999999998</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>41</v>
       </c>
@@ -1644,8 +2316,17 @@
       <c r="D75" s="2">
         <v>-9.7703010000000003E-3</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75" s="2">
+        <v>5.2383260000000001E-2</v>
+      </c>
+      <c r="F75" s="2">
+        <v>9.9722220000000004</v>
+      </c>
+      <c r="G75" s="2">
+        <v>-0.22531309999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>42</v>
       </c>
@@ -1658,8 +2339,17 @@
       <c r="D76" s="2">
         <v>3.8555699999999998E-2</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76" s="2">
+        <v>7.2916669999999999E-3</v>
+      </c>
+      <c r="F76" s="2">
+        <v>77</v>
+      </c>
+      <c r="G76" s="2">
+        <v>-3.9596810000000003E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>42</v>
       </c>
@@ -1672,8 +2362,17 @@
       <c r="D77" s="2">
         <v>-5.4751250000000001E-2</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" s="2">
+        <v>3.1820544999999999E-2</v>
+      </c>
+      <c r="F77" s="2">
+        <v>1.8455964300000001</v>
+      </c>
+      <c r="G77" s="2">
+        <v>-0.22658710000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>42</v>
       </c>
@@ -1686,8 +2385,17 @@
       <c r="D78" s="2">
         <v>4.2913399999999997E-2</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78" s="2">
+        <v>2.8925359999999998E-3</v>
+      </c>
+      <c r="F78" s="2">
+        <v>-6.4680440000000006E-2</v>
+      </c>
+      <c r="G78" s="2">
+        <v>6.7139669999999999E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>42</v>
       </c>
@@ -1700,8 +2408,17 @@
       <c r="D79" s="2">
         <v>-5.6139590000000003E-2</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79" s="2">
+        <v>1.1281493E-2</v>
+      </c>
+      <c r="F79" s="2">
+        <v>6.9837070000000001E-2</v>
+      </c>
+      <c r="G79" s="2">
+        <v>-7.4477749999999995E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>43</v>
       </c>
@@ -1714,8 +2431,17 @@
       <c r="D80" s="2">
         <v>0.21573629999999999</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80" s="2">
+        <v>2.4904368999999999E-2</v>
+      </c>
+      <c r="F80" s="2">
+        <v>12</v>
+      </c>
+      <c r="G80" s="2">
+        <v>0.2795107</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>43</v>
       </c>
@@ -1728,8 +2454,17 @@
       <c r="D81" s="2">
         <v>0.2158651</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81" s="2">
+        <v>6.064992E-3</v>
+      </c>
+      <c r="F81" s="2">
+        <v>-1.08054E-2</v>
+      </c>
+      <c r="G81" s="2">
+        <v>3.1096789999999999E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>44</v>
       </c>
@@ -1742,8 +2477,17 @@
       <c r="D82" s="2">
         <v>8.8029460000000004E-2</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82" s="2">
+        <v>6.7207790000000003E-2</v>
+      </c>
+      <c r="F82" s="2">
+        <v>9.2105263199999996</v>
+      </c>
+      <c r="G82" s="2">
+        <v>3.6641220000000002E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>44</v>
       </c>
@@ -1756,8 +2500,17 @@
       <c r="D83" s="2">
         <v>-5.2878139999999997E-2</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83" s="2">
+        <v>-0.16189442000000001</v>
+      </c>
+      <c r="F83" s="2">
+        <v>-2.2366819999999999E-2</v>
+      </c>
+      <c r="G83" s="2">
+        <v>-0.17941283</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>45</v>
       </c>
@@ -1770,8 +2523,17 @@
       <c r="D84" s="2">
         <v>-4.9406950000000002E-3</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84" s="2">
+        <v>7.0578975000000002E-2</v>
+      </c>
+      <c r="F84" s="2">
+        <v>3.1416122</v>
+      </c>
+      <c r="G84" s="2">
+        <v>-9.5682777999999996E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>45</v>
       </c>
@@ -1784,8 +2546,17 @@
       <c r="D85" s="2">
         <v>-3.6872756999999999E-2</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85" s="2">
+        <v>-3.5547281999999999E-2</v>
+      </c>
+      <c r="F85" s="2">
+        <v>0.12914884600000001</v>
+      </c>
+      <c r="G85" s="2">
+        <v>-9.0851620999999994E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>45</v>
       </c>
@@ -1798,8 +2569,17 @@
       <c r="D86" s="2">
         <v>3.0322897000000001E-2</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86" s="2">
+        <v>9.8019920000000007E-3</v>
+      </c>
+      <c r="F86" s="2">
+        <v>1.2408129999999999E-3</v>
+      </c>
+      <c r="G86" s="2">
+        <v>-4.221954E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>46</v>
       </c>
@@ -1812,8 +2592,17 @@
       <c r="D87" s="2">
         <v>3.5689650000000003E-2</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87" s="2">
+        <v>0.45302179999999997</v>
+      </c>
+      <c r="F87" s="2">
+        <v>1.2222219999999999</v>
+      </c>
+      <c r="G87" s="2">
+        <v>-0.33319769999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>47</v>
       </c>
@@ -1826,8 +2615,17 @@
       <c r="D88" s="2">
         <v>-2.4614960000000001E-3</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88" s="2">
+        <v>6.5951459999999996E-3</v>
+      </c>
+      <c r="F88" s="2">
+        <v>146.92857100000001</v>
+      </c>
+      <c r="G88" s="2">
+        <v>-0.23278070000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>47</v>
       </c>
@@ -1840,8 +2638,17 @@
       <c r="D89" s="2">
         <v>-4.9861276000000003E-2</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89" s="2">
+        <v>-3.1216206999999999E-2</v>
+      </c>
+      <c r="F89" s="2">
+        <v>1.366617</v>
+      </c>
+      <c r="G89" s="2">
+        <v>-0.47852879999999998</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>48</v>
       </c>
@@ -1854,8 +2661,17 @@
       <c r="D90" s="2">
         <v>7.5764899999999996E-2</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E90" s="2">
+        <v>2.5871060000000001E-2</v>
+      </c>
+      <c r="F90" s="2">
+        <v>9.1176469999999998</v>
+      </c>
+      <c r="G90" s="2">
+        <v>-7.0050059999999997E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>49</v>
       </c>
@@ -1868,8 +2684,17 @@
       <c r="D91" s="2">
         <v>4.8824949999999999E-2</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E91" s="2">
+        <v>6.7567570000000004E-3</v>
+      </c>
+      <c r="F91" s="2">
+        <v>0.86666670000000001</v>
+      </c>
+      <c r="G91" s="2">
+        <v>-0.37155569999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>50</v>
       </c>
@@ -1882,8 +2707,17 @@
       <c r="D92" s="2">
         <v>6.2783500000000006E-2</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E92" s="2">
+        <v>4.5092220000000002E-2</v>
+      </c>
+      <c r="F92" s="2">
+        <v>53</v>
+      </c>
+      <c r="G92" s="2">
+        <v>0.73594510000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>51</v>
       </c>
@@ -1896,8 +2730,17 @@
       <c r="D93" s="2">
         <v>8.2228369999999995E-2</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E93" s="2">
+        <v>7.3832903000000005E-2</v>
+      </c>
+      <c r="F93" s="2">
+        <v>10</v>
+      </c>
+      <c r="G93" s="2">
+        <v>-0.107616932</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>51</v>
       </c>
@@ -1910,16 +2753,30 @@
       <c r="D94" s="2">
         <v>4.0459380000000003E-2</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+      <c r="E94" s="2">
+        <v>-4.2490380000000001E-3</v>
+      </c>
+      <c r="F94" s="2">
+        <v>1.738025E-2</v>
+      </c>
+      <c r="G94" s="2">
+        <v>1.995344E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="14">
         <v>43556</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C95" s="13"/>
+      <c r="D95" s="15"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="15"/>
+      <c r="G95" s="15"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>52</v>
       </c>
@@ -1932,8 +2789,17 @@
       <c r="D96" s="2">
         <v>-2.8176429999999999E-2</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E96" s="2">
+        <v>1.06383E-3</v>
+      </c>
+      <c r="F96" s="2">
+        <v>23</v>
+      </c>
+      <c r="G96" s="2">
+        <v>-6.5773319999999996E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>52</v>
       </c>
@@ -1946,8 +2812,17 @@
       <c r="D97" s="2">
         <v>-2.9144199999999999E-2</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E97" s="2">
+        <v>1.105895E-2</v>
+      </c>
+      <c r="F97" s="2">
+        <v>0.70558739999999998</v>
+      </c>
+      <c r="G97" s="2">
+        <v>-1.525229E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>53</v>
       </c>
@@ -1960,8 +2835,17 @@
       <c r="D98" s="2">
         <v>0.1140298</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98" s="2">
+        <v>-3.3849980000000002E-2</v>
+      </c>
+      <c r="F98" s="2">
+        <v>6.3333329999999997</v>
+      </c>
+      <c r="G98" s="2">
+        <v>-0.37554739999999998</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>54</v>
       </c>
@@ -1974,8 +2858,17 @@
       <c r="D99" s="2">
         <v>-3.2172720000000002E-3</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99" s="2">
+        <v>3.2517840000000002E-3</v>
+      </c>
+      <c r="F99" s="2">
+        <v>0.73269229999999996</v>
+      </c>
+      <c r="G99" s="2">
+        <v>8.3974439999999997E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="8" t="s">
         <v>55</v>
       </c>
@@ -1988,10 +2881,19 @@
       <c r="D100" s="10">
         <v>3.172705E-2</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E100" s="2">
+        <v>1.9751500000000002E-2</v>
+      </c>
+      <c r="F100" s="2">
+        <v>0.2428786</v>
+      </c>
+      <c r="G100" s="2">
+        <v>-9.3543580000000001E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="11" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>